<commit_message>
Added tests to Leadimage
</commit_message>
<xml_diff>
--- a/test-data/leadimage-data.xlsx
+++ b/test-data/leadimage-data.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cgov_workspace\cgov-digital-platform-qa\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B19B72-CD38-40B2-916A-7B5C21ED1203}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B129ED4-100A-4C84-BD84-2DDB08C8D813}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4280" yWindow="2760" windowWidth="14930" windowHeight="5460" activeTab="1" xr2:uid="{112BCE41-1B7B-AF44-BEF2-07A92CFC037C}"/>
+    <workbookView minimized="1" xWindow="4280" yWindow="2760" windowWidth="14920" windowHeight="5460" activeTab="4" xr2:uid="{112BCE41-1B7B-AF44-BEF2-07A92CFC037C}"/>
   </bookViews>
   <sheets>
     <sheet name="pages_with_leadimage" sheetId="1" r:id="rId1"/>
     <sheet name="pages_with_noleadimage" sheetId="5" r:id="rId2"/>
+    <sheet name="pages_with_leadimage_Alt" sheetId="7" r:id="rId3"/>
+    <sheet name="pages_with_leadimage_Credit" sheetId="8" r:id="rId4"/>
+    <sheet name="pages_with_leadimage_Caption" sheetId="9" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="42">
   <si>
     <t>path</t>
   </si>
@@ -85,9 +89,6 @@
     <t>Alt text</t>
   </si>
   <si>
-    <t>Oncol Letters Jan 2016. doi: 10.3892/ol.2015.3906 CC BY 4.0.</t>
-  </si>
-  <si>
     <t>A CT scan of a tumor in the right femur of a woman with alveolar soft part sarcoma.</t>
   </si>
   <si>
@@ -100,18 +101,12 @@
     <t>Sad Woman Looking Out Window</t>
   </si>
   <si>
-    <t>iStock</t>
-  </si>
-  <si>
     <t>Circos plot shows data from The Cancer Genome Atlas (TCGA)</t>
   </si>
   <si>
     <t>This Circos plot visualizes data from The Cancer Genome Atlas (TCGA) and allows scientists to explore the interrelationships among different data points.</t>
   </si>
   <si>
-    <t>National Cancer Institute</t>
-  </si>
-  <si>
     <t>news-events/press-releases/2019/annual-report-nation-2018</t>
   </si>
   <si>
@@ -127,9 +122,6 @@
     <t>El diagrama de Circos visualiza datos del Atlas del Genoma de Cáncer (TCGA) y permite a los científicos explorar las interrelaciones entre los puntos diferentes de datos.</t>
   </si>
   <si>
-    <t>Instituto Nacional del Cáncer</t>
-  </si>
-  <si>
     <t>about-cancer/coping/feelings/relaxation/stress-fact-sheet</t>
   </si>
   <si>
@@ -143,6 +135,27 @@
   </si>
   <si>
     <t>research/key-initiatives/ras/ras-central/blog/2017/ras-dependent</t>
+  </si>
+  <si>
+    <t>Credit: National Cancer Institute</t>
+  </si>
+  <si>
+    <t>Credit: Instituto Nacional del Cáncer</t>
+  </si>
+  <si>
+    <t>Credit: Oncol Letters Jan 2016. doi: 10.3892/ol.2015.3906 CC BY 4.0.</t>
+  </si>
+  <si>
+    <t>Credit: iStock</t>
+  </si>
+  <si>
+    <t>news-events/press-releases/2019/brca-exchange</t>
+  </si>
+  <si>
+    <t>The BRXA Exhange graphic</t>
+  </si>
+  <si>
+    <t>Credit: BRCA Challenge</t>
   </si>
 </sst>
 </file>
@@ -497,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ABDEF67-3BF3-604C-97A8-A43819B8E79D}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -541,18 +554,18 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -561,92 +574,13 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
         <v>28</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -658,8 +592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26668E1C-E236-40F0-B5CF-1CC4E870A494}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -682,7 +616,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -704,7 +638,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -715,7 +649,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -726,7 +660,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -737,13 +671,437 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28FD5B02-F1AB-4576-A73A-244C78D6C857}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="66.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="5" max="5" width="28.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74DB49F4-0D71-45D4-8B24-7BA34D48B26C}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="58.1640625" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="57.08203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58FE319F-68B5-4879-B9F9-8C755E7FDE1F}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="58.1640625" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="57.08203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2BE01AF-FEF7-4210-A6FF-8402CF9BF4C6}">
+  <dimension ref="A2:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Test Case: Verify Lead Image #17
</commit_message>
<xml_diff>
--- a/test-data/leadimage-data.xlsx
+++ b/test-data/leadimage-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cgov_workspace\cgov-digital-platform-qa\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C297D252-1822-47FA-AC41-3FCBEA9C0B16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45512A95-66D2-48FC-9B31-8E4EA781D466}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="2760" windowWidth="14925" windowHeight="5460" firstSheet="3" activeTab="4" xr2:uid="{112BCE41-1B7B-AF44-BEF2-07A92CFC037C}"/>
+    <workbookView xWindow="4280" yWindow="2760" windowWidth="14930" windowHeight="5460" firstSheet="2" activeTab="4" xr2:uid="{112BCE41-1B7B-AF44-BEF2-07A92CFC037C}"/>
   </bookViews>
   <sheets>
     <sheet name="pages_with_leadimage" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="47">
   <si>
     <t>path</t>
   </si>
@@ -143,6 +143,33 @@
   </si>
   <si>
     <t>Credit: BRCA Challenge</t>
+  </si>
+  <si>
+    <t>espanol/efectos-secundarios</t>
+  </si>
+  <si>
+    <t>Reconstrucción</t>
+  </si>
+  <si>
+    <t>Los implantes se insertan debajo de la piel o del músculo del pecho</t>
+  </si>
+  <si>
+    <t>about-cancer/treatment/side-effects</t>
+  </si>
+  <si>
+    <t>Tell your doctor about side effects you are experiencing, so you get the care and treatment you need to manage these problems.</t>
+  </si>
+  <si>
+    <t>Reconstruction</t>
+  </si>
+  <si>
+    <t>news-events/press-releases/2018/leukemia-cll-ibrutinib-trial</t>
+  </si>
+  <si>
+    <t>Ibrutinib plus rituximab superior to standard treatment for some patients with chronic leukemia</t>
+  </si>
+  <si>
+    <t>patients with chronic leukemia</t>
   </si>
 </sst>
 </file>
@@ -497,20 +524,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ABDEF67-3BF3-604C-97A8-A43819B8E79D}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="66.375" customWidth="1"/>
+    <col min="1" max="1" width="66.33203125" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="3" width="9.875" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -530,7 +557,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -550,7 +577,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -568,6 +595,66 @@
       </c>
       <c r="F3" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -583,14 +670,14 @@
       <selection activeCell="A5" sqref="A5:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="66.375" customWidth="1"/>
+    <col min="1" max="1" width="66.33203125" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="3" width="9.875" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -601,7 +688,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -612,7 +699,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -623,7 +710,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -634,7 +721,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -645,7 +732,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -656,7 +743,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -674,21 +761,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28FD5B02-F1AB-4576-A73A-244C78D6C857}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="66.375" customWidth="1"/>
+    <col min="1" max="1" width="66.33203125" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="3" width="9.875" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
     <col min="5" max="5" width="28.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -708,7 +795,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -728,7 +815,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -748,7 +835,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -765,7 +852,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -782,7 +869,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -797,6 +884,66 @@
       </c>
       <c r="F6" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -806,22 +953,22 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74DB49F4-0D71-45D4-8B24-7BA34D48B26C}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="58.125" customWidth="1"/>
+    <col min="1" max="1" width="58.08203125" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="3" width="9.875" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="57.125" customWidth="1"/>
+    <col min="5" max="5" width="57.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -841,7 +988,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -858,7 +1005,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -878,7 +1025,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -898,7 +1045,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -915,7 +1062,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -932,7 +1079,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -947,6 +1094,66 @@
       </c>
       <c r="F7" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -956,22 +1163,22 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58FE319F-68B5-4879-B9F9-8C755E7FDE1F}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="58.125" customWidth="1"/>
+    <col min="1" max="1" width="58.08203125" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="3" width="9.875" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="57.125" customWidth="1"/>
+    <col min="5" max="5" width="57.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -991,7 +1198,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1011,7 +1218,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1029,6 +1236,46 @@
       </c>
       <c r="F3" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>